<commit_message>
Added Window Application Script
</commit_message>
<xml_diff>
--- a/Scenario_Control.xlsx
+++ b/Scenario_Control.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\UFT Framework Experiment\Enhanced\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\UFT Framework Enhanced\Enhanced-UFT-Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAB946F-B7A6-46A2-9756-AD7C72E7D567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62107A76-2C14-4F8C-8A05-C882A31CDBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Module_Folder_Name</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>AOS_IOS_Register_01</t>
+  </si>
+  <si>
+    <t>Book Flights</t>
+  </si>
+  <si>
+    <t>Select_Destination</t>
+  </si>
+  <si>
+    <t>Test1Flight</t>
+  </si>
+  <si>
+    <t>Verify booking flights successfully</t>
   </si>
 </sst>
 </file>
@@ -533,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +836,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -842,7 +854,7 @@
         <v>31</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -860,7 +872,7 @@
         <v>32</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -880,7 +892,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -898,7 +910,7 @@
         <v>40</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -909,6 +921,44 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed scrollintoview and scrollby functions to another function library WebObjectAction.qfl
</commit_message>
<xml_diff>
--- a/Scenario_Control.xlsx
+++ b/Scenario_Control.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\UFT Framework Enhanced\Enhanced-UFT-Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940016F9-F07F-4B4C-B8EA-B12360951EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A4B40-01C3-40EC-8946-B776A2A626D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Module_Folder_Name</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>Verify booking flights successfully</t>
-  </si>
-  <si>
-    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -551,7 +548,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +590,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -611,7 +608,7 @@
         <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -649,7 +646,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -667,7 +664,7 @@
         <v>51</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -895,7 +892,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -913,7 +910,7 @@
         <v>40</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified WebObjectAction.qfl VerifyText and VerifyTextContains Function to handle error prompt by UFT One if the object ID is incorrect
</commit_message>
<xml_diff>
--- a/Scenario_Control.xlsx
+++ b/Scenario_Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\UFT Framework Enhanced\Enhanced-UFT-Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A4B40-01C3-40EC-8946-B776A2A626D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CBA5AB-1DFC-469C-A0DD-36D6D7BC7EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="F25" sqref="F24:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>36</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>